<commit_message>
Initial commit: Snag and project management app
</commit_message>
<xml_diff>
--- a/Steps.xlsx
+++ b/Steps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://specconsa-my.sharepoint.com/personal/hein_speccon_co_za/Documents/Software Development/Projects v2/Snag List and Project Management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF42E0C1-5B32-40F6-8D95-9E7C87A6EBCF}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8B9C4AC-E793-4ADC-87CD-14ED1CEEE9C1}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="42930" yWindow="2595" windowWidth="19200" windowHeight="9975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Idea on notepad</t>
   </si>
@@ -854,6 +854,12 @@
   </si>
   <si>
     <t>Build and deploy</t>
+  </si>
+  <si>
+    <t>Deploy to Github first, then to Google console</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> npm ci</t>
   </si>
 </sst>
 </file>
@@ -1380,7 +1386,7 @@
   <dimension ref="A1:C86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.5" x14ac:dyDescent="0.55000000000000004"/>
@@ -1752,65 +1758,71 @@
         <v>76</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="4"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B76" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B78" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="4" t="s">
         <v>58</v>
       </c>

</xml_diff>